<commit_message>
add checking to tabulator tables for CRJ
</commit_message>
<xml_diff>
--- a/Documents/ACCOUNTING EQUATION TEMPLATE.xlsx
+++ b/Documents/ACCOUNTING EQUATION TEMPLATE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydnicholson/Documents/GitHub/accounting-app/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D100F3E9-7F11-F04D-9DC9-7C70BFDA3DB6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F55D6F7-B5CF-C547-82EF-D338C72CD3B4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{FA2973F7-7B77-A140-8E17-44680C9A4F59}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="20480" xr2:uid="{FA2973F7-7B77-A140-8E17-44680C9A4F59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
   <dimension ref="B2:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="224" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,7 +523,6 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>

</xml_diff>

<commit_message>
add new files for testing and create new collapse fixed top nav
</commit_message>
<xml_diff>
--- a/Documents/ACCOUNTING EQUATION TEMPLATE.xlsx
+++ b/Documents/ACCOUNTING EQUATION TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydnicholson/Documents/GitHub/accounting-app/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F55D6F7-B5CF-C547-82EF-D338C72CD3B4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07983D49-48A5-444B-9CA6-16E9CF0E703A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="20480" xr2:uid="{FA2973F7-7B77-A140-8E17-44680C9A4F59}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="17540" xr2:uid="{FA2973F7-7B77-A140-8E17-44680C9A4F59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,12 +105,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +429,7 @@
   <dimension ref="B2:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="224" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,6 +524,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
@@ -664,9 +666,9 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
@@ -674,9 +676,9 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
@@ -684,9 +686,9 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
@@ -694,9 +696,9 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
@@ -704,9 +706,9 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
@@ -714,9 +716,9 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>